<commit_message>
shiro database query privilege
</commit_message>
<xml_diff>
--- a/src/main/resources/backup/Yr 1 report weeks 1-3 Autumn 2015.xlsx
+++ b/src/main/resources/backup/Yr 1 report weeks 1-3 Autumn 2015.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\final_year_project\spring-boot-project\src\main\resources\backup\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16095" windowHeight="25650" tabRatio="500"/>
+    <workbookView windowHeight="18450" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97">
   <si>
     <t>Lvl</t>
   </si>
@@ -317,16 +312,173 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,12 +493,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -369,9 +707,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -384,17 +964,61 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -716,37 +1340,37 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="7.33333333333333" customWidth="1"/>
+    <col min="2" max="2" width="11.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="12.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="25.8888888888889" customWidth="1"/>
+    <col min="7" max="7" width="11.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="8.55555555555556" customWidth="1"/>
+    <col min="9" max="9" width="17.1111111111111" customWidth="1"/>
+    <col min="10" max="10" width="8.88888888888889" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1"/>
-    <col min="16" max="16" width="20.88671875" customWidth="1"/>
-    <col min="17" max="17" width="58.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.1111111111111" customWidth="1"/>
+    <col min="13" max="13" width="15.5555555555556" customWidth="1"/>
+    <col min="14" max="14" width="17.8888888888889" customWidth="1"/>
+    <col min="15" max="15" width="12.4444444444444" customWidth="1"/>
+    <col min="16" max="16" width="20.8888888888889" customWidth="1"/>
+    <col min="17" max="17" width="58.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -845,7 +1469,7 @@
         <v>22</v>
       </c>
       <c r="P2" s="6">
-        <v>42271.666666666701</v>
+        <v>42271.6666666667</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>23</v>
@@ -894,7 +1518,7 @@
         <v>22</v>
       </c>
       <c r="P3" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q3" s="2"/>
     </row>
@@ -945,7 +1569,7 @@
         <v>22</v>
       </c>
       <c r="P4" s="6">
-        <v>42278.666666666701</v>
+        <v>42278.6666666667</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>29</v>
@@ -983,7 +1607,7 @@
         <v>21</v>
       </c>
       <c r="K5" s="4">
-        <v>0.76200000000000001</v>
+        <v>0.762</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -994,7 +1618,7 @@
         <v>22</v>
       </c>
       <c r="P5" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q5" s="2"/>
     </row>
@@ -1030,7 +1654,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="4">
-        <v>0.78600000000000003</v>
+        <v>0.786</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1041,7 +1665,7 @@
         <v>34</v>
       </c>
       <c r="P6" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>35</v>
@@ -1079,7 +1703,7 @@
         <v>18</v>
       </c>
       <c r="K7" s="4">
-        <v>0.61099999999999999</v>
+        <v>0.611</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1090,7 +1714,7 @@
         <v>22</v>
       </c>
       <c r="P7" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>36</v>
@@ -1128,7 +1752,7 @@
         <v>20</v>
       </c>
       <c r="K8" s="4">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1139,7 +1763,7 @@
         <v>22</v>
       </c>
       <c r="P8" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q8" s="2"/>
     </row>
@@ -1220,7 +1844,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="4">
-        <v>0.28599999999999998</v>
+        <v>0.286</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1267,7 +1891,7 @@
         <v>19</v>
       </c>
       <c r="K11" s="4">
-        <v>0.52600000000000002</v>
+        <v>0.526</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1278,7 +1902,7 @@
         <v>22</v>
       </c>
       <c r="P11" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q11" s="2"/>
     </row>
@@ -1314,7 +1938,7 @@
         <v>19</v>
       </c>
       <c r="K12" s="4">
-        <v>0.52600000000000002</v>
+        <v>0.526</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1325,7 +1949,7 @@
         <v>22</v>
       </c>
       <c r="P12" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q12" s="2"/>
     </row>
@@ -1419,7 +2043,7 @@
         <v>34</v>
       </c>
       <c r="P14" s="6">
-        <v>42276.541666666701</v>
+        <v>42276.5416666667</v>
       </c>
       <c r="Q14" s="2"/>
     </row>
@@ -1466,11 +2090,11 @@
         <v>34</v>
       </c>
       <c r="P15" s="6">
-        <v>42279.583333333299</v>
+        <v>42279.5833333333</v>
       </c>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" s="1" customFormat="1">
+    <row r="16" s="1" customFormat="1" spans="1:17">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1547,7 +2171,7 @@
         <v>14</v>
       </c>
       <c r="K17" s="4">
-        <v>0.64300000000000002</v>
+        <v>0.643</v>
       </c>
       <c r="L17" s="7">
         <v>42264</v>
@@ -1562,7 +2186,7 @@
         <v>34</v>
       </c>
       <c r="P17" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q17" s="2"/>
     </row>
@@ -1598,7 +2222,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="4">
-        <v>0.78600000000000003</v>
+        <v>0.786</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1609,7 +2233,7 @@
         <v>34</v>
       </c>
       <c r="P18" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q18" s="2"/>
     </row>
@@ -1645,7 +2269,7 @@
         <v>14</v>
       </c>
       <c r="K19" s="4">
-        <v>0.78600000000000003</v>
+        <v>0.786</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1656,7 +2280,7 @@
         <v>34</v>
       </c>
       <c r="P19" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q19" s="2"/>
     </row>
@@ -1692,7 +2316,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="4">
-        <v>0.28599999999999998</v>
+        <v>0.286</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1739,7 +2363,7 @@
         <v>14</v>
       </c>
       <c r="K21" s="4">
-        <v>0.78600000000000003</v>
+        <v>0.786</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1750,7 +2374,7 @@
         <v>34</v>
       </c>
       <c r="P21" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q21" s="2"/>
     </row>
@@ -1786,7 +2410,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="4">
-        <v>0.78600000000000003</v>
+        <v>0.786</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1797,7 +2421,7 @@
         <v>34</v>
       </c>
       <c r="P22" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q22" s="2"/>
     </row>
@@ -1833,7 +2457,7 @@
         <v>14</v>
       </c>
       <c r="K23" s="4">
-        <v>0.71399999999999997</v>
+        <v>0.714</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1844,7 +2468,7 @@
         <v>22</v>
       </c>
       <c r="P23" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>48</v>
@@ -1882,7 +2506,7 @@
         <v>12</v>
       </c>
       <c r="K24" s="4">
-        <v>0.58299999999999996</v>
+        <v>0.583</v>
       </c>
       <c r="L24" s="7">
         <v>42263</v>
@@ -1944,7 +2568,7 @@
         <v>34</v>
       </c>
       <c r="P25" s="6">
-        <v>42278.541666666701</v>
+        <v>42278.5416666667</v>
       </c>
       <c r="Q25" s="2"/>
     </row>
@@ -1980,7 +2604,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="4">
-        <v>0.71399999999999997</v>
+        <v>0.714</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -1991,7 +2615,7 @@
         <v>34</v>
       </c>
       <c r="P26" s="6">
-        <v>42278.583333333299</v>
+        <v>42278.5833333333</v>
       </c>
       <c r="Q26" s="2"/>
     </row>
@@ -2027,7 +2651,7 @@
         <v>12</v>
       </c>
       <c r="K27" s="4">
-        <v>0.66700000000000004</v>
+        <v>0.667</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -2038,7 +2662,7 @@
         <v>34</v>
       </c>
       <c r="P27" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q27" s="2"/>
     </row>
@@ -2074,7 +2698,7 @@
         <v>14</v>
       </c>
       <c r="K28" s="4">
-        <v>0.57099999999999995</v>
+        <v>0.571</v>
       </c>
       <c r="L28" s="7">
         <v>42264</v>
@@ -2089,7 +2713,7 @@
         <v>34</v>
       </c>
       <c r="P28" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q28" s="2"/>
     </row>
@@ -2275,7 +2899,7 @@
         <v>34</v>
       </c>
       <c r="P32" s="6">
-        <v>42271.666666666701</v>
+        <v>42271.6666666667</v>
       </c>
       <c r="Q32" s="2"/>
     </row>
@@ -2311,7 +2935,7 @@
         <v>12</v>
       </c>
       <c r="K33" s="4">
-        <v>0.58299999999999996</v>
+        <v>0.583</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -2456,7 +3080,7 @@
         <v>18</v>
       </c>
       <c r="K36" s="4">
-        <v>5.6000000000000001E-2</v>
+        <v>0.056</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -2467,7 +3091,7 @@
         <v>34</v>
       </c>
       <c r="P36" s="6">
-        <v>42272.541666666701</v>
+        <v>42272.5416666667</v>
       </c>
       <c r="Q36" s="2"/>
     </row>
@@ -2503,7 +3127,7 @@
         <v>14</v>
       </c>
       <c r="K37" s="4">
-        <v>0.78600000000000003</v>
+        <v>0.786</v>
       </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
@@ -2550,7 +3174,7 @@
         <v>15</v>
       </c>
       <c r="K38" s="4">
-        <v>6.7000000000000004E-2</v>
+        <v>0.067</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
@@ -2561,7 +3185,7 @@
         <v>34</v>
       </c>
       <c r="P38" s="6">
-        <v>42269.458333333299</v>
+        <v>42269.4583333333</v>
       </c>
       <c r="Q38" s="2"/>
     </row>
@@ -2608,7 +3232,7 @@
         <v>34</v>
       </c>
       <c r="P39" s="6">
-        <v>42278.583333333299</v>
+        <v>42278.5833333333</v>
       </c>
       <c r="Q39" s="2"/>
     </row>
@@ -2655,7 +3279,7 @@
         <v>22</v>
       </c>
       <c r="P40" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q40" s="2"/>
     </row>
@@ -2702,7 +3326,7 @@
         <v>34</v>
       </c>
       <c r="P41" s="6">
-        <v>42278.458333333299</v>
+        <v>42278.4583333333</v>
       </c>
       <c r="Q41" s="2"/>
     </row>
@@ -2798,7 +3422,7 @@
         <v>34</v>
       </c>
       <c r="P43" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q43" s="2"/>
     </row>
@@ -2834,7 +3458,7 @@
         <v>14</v>
       </c>
       <c r="K44" s="4">
-        <v>0.57099999999999995</v>
+        <v>0.571</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
@@ -2845,7 +3469,7 @@
         <v>34</v>
       </c>
       <c r="P44" s="6">
-        <v>42278.583333333299</v>
+        <v>42278.5833333333</v>
       </c>
       <c r="Q44" s="2"/>
     </row>
@@ -2881,7 +3505,7 @@
         <v>14</v>
       </c>
       <c r="K45" s="4">
-        <v>0.42899999999999999</v>
+        <v>0.429</v>
       </c>
       <c r="L45" s="7">
         <v>42213</v>
@@ -2896,11 +3520,11 @@
         <v>34</v>
       </c>
       <c r="P45" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" s="1" customFormat="1">
+    <row r="46" s="1" customFormat="1" spans="1:17">
       <c r="A46" s="3" t="s">
         <v>17</v>
       </c>
@@ -2977,7 +3601,7 @@
         <v>19</v>
       </c>
       <c r="K47" s="4">
-        <v>0.68400000000000005</v>
+        <v>0.684</v>
       </c>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
@@ -2988,7 +3612,7 @@
         <v>34</v>
       </c>
       <c r="P47" s="6">
-        <v>42279.583333333299</v>
+        <v>42279.5833333333</v>
       </c>
       <c r="Q47" s="2"/>
     </row>
@@ -3024,7 +3648,7 @@
         <v>14</v>
       </c>
       <c r="K48" s="4">
-        <v>0.42899999999999999</v>
+        <v>0.429</v>
       </c>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
@@ -3071,7 +3695,7 @@
         <v>12</v>
       </c>
       <c r="K49" s="4">
-        <v>0.41699999999999998</v>
+        <v>0.417</v>
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
@@ -3082,7 +3706,7 @@
         <v>22</v>
       </c>
       <c r="P49" s="6">
-        <v>42272.541666666701</v>
+        <v>42272.5416666667</v>
       </c>
       <c r="Q49" s="2"/>
     </row>
@@ -3129,7 +3753,7 @@
         <v>34</v>
       </c>
       <c r="P50" s="6">
-        <v>42278.666666666701</v>
+        <v>42278.6666666667</v>
       </c>
       <c r="Q50" s="2"/>
     </row>
@@ -3165,7 +3789,7 @@
         <v>14</v>
       </c>
       <c r="K51" s="4">
-        <v>0.71399999999999997</v>
+        <v>0.714</v>
       </c>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
@@ -3176,7 +3800,7 @@
         <v>34</v>
       </c>
       <c r="P51" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q51" s="2"/>
     </row>
@@ -3223,7 +3847,7 @@
         <v>34</v>
       </c>
       <c r="P52" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q52" s="2"/>
     </row>
@@ -3259,7 +3883,7 @@
         <v>15</v>
       </c>
       <c r="K53" s="4">
-        <v>0.66700000000000004</v>
+        <v>0.667</v>
       </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
@@ -3270,7 +3894,7 @@
         <v>34</v>
       </c>
       <c r="P53" s="6">
-        <v>42278.666666666701</v>
+        <v>42278.6666666667</v>
       </c>
       <c r="Q53" s="2"/>
     </row>
@@ -3317,7 +3941,7 @@
         <v>22</v>
       </c>
       <c r="P54" s="6">
-        <v>42276.541666666701</v>
+        <v>42276.5416666667</v>
       </c>
       <c r="Q54" s="2"/>
     </row>
@@ -3353,7 +3977,7 @@
         <v>14</v>
       </c>
       <c r="K55" s="4">
-        <v>0.28599999999999998</v>
+        <v>0.286</v>
       </c>
       <c r="L55" s="7">
         <v>42278</v>
@@ -3368,7 +3992,7 @@
         <v>22</v>
       </c>
       <c r="P55" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q55" s="2"/>
     </row>
@@ -3404,7 +4028,7 @@
         <v>14</v>
       </c>
       <c r="K56" s="4">
-        <v>0.78600000000000003</v>
+        <v>0.786</v>
       </c>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
@@ -3453,7 +4077,7 @@
         <v>14</v>
       </c>
       <c r="K57" s="4">
-        <v>0.71399999999999997</v>
+        <v>0.714</v>
       </c>
       <c r="L57" s="7">
         <v>42277</v>
@@ -3468,7 +4092,7 @@
         <v>34</v>
       </c>
       <c r="P57" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q57" s="2"/>
     </row>
@@ -3504,7 +4128,7 @@
         <v>14</v>
       </c>
       <c r="K58" s="4">
-        <v>0.42899999999999999</v>
+        <v>0.429</v>
       </c>
       <c r="L58" s="7">
         <v>42279</v>
@@ -3557,7 +4181,7 @@
         <v>21</v>
       </c>
       <c r="K59" s="4">
-        <v>0.47599999999999998</v>
+        <v>0.476</v>
       </c>
       <c r="L59" s="7">
         <v>42236</v>
@@ -3625,7 +4249,7 @@
         <v>22</v>
       </c>
       <c r="P60" s="6">
-        <v>42269.458333333299</v>
+        <v>42269.4583333333</v>
       </c>
       <c r="Q60" s="2"/>
     </row>
@@ -3672,7 +4296,7 @@
         <v>34</v>
       </c>
       <c r="P61" s="6">
-        <v>42279.583333333299</v>
+        <v>42279.5833333333</v>
       </c>
       <c r="Q61" s="2"/>
     </row>
@@ -3708,7 +4332,7 @@
         <v>19</v>
       </c>
       <c r="K62" s="4">
-        <v>0.78900000000000003</v>
+        <v>0.789</v>
       </c>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
@@ -3719,7 +4343,7 @@
         <v>34</v>
       </c>
       <c r="P62" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q62" s="2"/>
     </row>
@@ -3755,7 +4379,7 @@
         <v>14</v>
       </c>
       <c r="K63" s="4">
-        <v>0.78600000000000003</v>
+        <v>0.786</v>
       </c>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -3766,7 +4390,7 @@
         <v>34</v>
       </c>
       <c r="P63" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q63" s="2"/>
     </row>
@@ -3802,7 +4426,7 @@
         <v>12</v>
       </c>
       <c r="K64" s="4">
-        <v>0.66700000000000004</v>
+        <v>0.667</v>
       </c>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
@@ -3813,7 +4437,7 @@
         <v>34</v>
       </c>
       <c r="P64" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q64" s="2"/>
     </row>
@@ -3860,7 +4484,7 @@
         <v>34</v>
       </c>
       <c r="P65" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q65" s="2"/>
     </row>
@@ -3896,7 +4520,7 @@
         <v>12</v>
       </c>
       <c r="K66" s="4">
-        <v>0.66700000000000004</v>
+        <v>0.667</v>
       </c>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
@@ -3907,7 +4531,7 @@
         <v>34</v>
       </c>
       <c r="P66" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q66" s="2"/>
     </row>
@@ -3943,7 +4567,7 @@
         <v>14</v>
       </c>
       <c r="K67" s="4">
-        <v>0.71399999999999997</v>
+        <v>0.714</v>
       </c>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
@@ -3954,7 +4578,7 @@
         <v>34</v>
       </c>
       <c r="P67" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q67" s="2"/>
     </row>
@@ -3990,7 +4614,7 @@
         <v>14</v>
       </c>
       <c r="K68" s="4">
-        <v>0.64300000000000002</v>
+        <v>0.643</v>
       </c>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
@@ -4048,7 +4672,7 @@
         <v>34</v>
       </c>
       <c r="P69" s="6">
-        <v>42278.666666666701</v>
+        <v>42278.6666666667</v>
       </c>
       <c r="Q69" s="2"/>
     </row>
@@ -4084,7 +4708,7 @@
         <v>14</v>
       </c>
       <c r="K70" s="4">
-        <v>0.64300000000000002</v>
+        <v>0.643</v>
       </c>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
@@ -4142,7 +4766,7 @@
         <v>34</v>
       </c>
       <c r="P71" s="6">
-        <v>42272.541666666701</v>
+        <v>42272.5416666667</v>
       </c>
       <c r="Q71" s="2"/>
     </row>
@@ -4315,7 +4939,7 @@
         <v>19</v>
       </c>
       <c r="K75" s="4">
-        <v>0.42099999999999999</v>
+        <v>0.421</v>
       </c>
       <c r="L75" s="7">
         <v>42258</v>
@@ -4556,7 +5180,7 @@
         <v>18</v>
       </c>
       <c r="K80" s="4">
-        <v>0.44400000000000001</v>
+        <v>0.444</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
@@ -4567,7 +5191,7 @@
         <v>34</v>
       </c>
       <c r="P80" s="6">
-        <v>42272.583333333299</v>
+        <v>42272.5833333333</v>
       </c>
       <c r="Q80" s="2"/>
     </row>
@@ -4603,7 +5227,7 @@
         <v>14</v>
       </c>
       <c r="K81" s="4">
-        <v>0.64300000000000002</v>
+        <v>0.643</v>
       </c>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
@@ -4614,7 +5238,7 @@
         <v>34</v>
       </c>
       <c r="P81" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q81" s="2"/>
     </row>
@@ -4650,7 +5274,7 @@
         <v>16</v>
       </c>
       <c r="K82" s="4">
-        <v>0.56299999999999994</v>
+        <v>0.563</v>
       </c>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
@@ -4661,7 +5285,7 @@
         <v>34</v>
       </c>
       <c r="P82" s="6">
-        <v>42276.541666666701</v>
+        <v>42276.5416666667</v>
       </c>
       <c r="Q82" s="2"/>
     </row>
@@ -4697,7 +5321,7 @@
         <v>18</v>
       </c>
       <c r="K83" s="4">
-        <v>5.6000000000000001E-2</v>
+        <v>0.056</v>
       </c>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
@@ -4708,7 +5332,7 @@
         <v>22</v>
       </c>
       <c r="P83" s="6">
-        <v>42269.458333333299</v>
+        <v>42269.4583333333</v>
       </c>
       <c r="Q83" s="2"/>
     </row>
@@ -4744,7 +5368,7 @@
         <v>14</v>
       </c>
       <c r="K84" s="4">
-        <v>0.64300000000000002</v>
+        <v>0.643</v>
       </c>
       <c r="L84" s="7">
         <v>41912</v>
@@ -4795,7 +5419,7 @@
         <v>14</v>
       </c>
       <c r="K85" s="4">
-        <v>0.14299999999999999</v>
+        <v>0.143</v>
       </c>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
@@ -4806,7 +5430,7 @@
         <v>34</v>
       </c>
       <c r="P85" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q85" s="2" t="s">
         <v>93</v>
@@ -4855,7 +5479,7 @@
         <v>34</v>
       </c>
       <c r="P86" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q86" s="2"/>
     </row>
@@ -4902,7 +5526,7 @@
         <v>34</v>
       </c>
       <c r="P87" s="6">
-        <v>42279.541666666701</v>
+        <v>42279.5416666667</v>
       </c>
       <c r="Q87" s="2"/>
     </row>
@@ -4938,7 +5562,7 @@
         <v>12</v>
       </c>
       <c r="K88" s="4">
-        <v>0.66700000000000004</v>
+        <v>0.667</v>
       </c>
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
@@ -4949,11 +5573,11 @@
         <v>22</v>
       </c>
       <c r="P88" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q88" s="2"/>
     </row>
-    <row r="89" spans="1:17" s="1" customFormat="1">
+    <row r="89" s="1" customFormat="1" spans="1:17">
       <c r="A89" s="3" t="s">
         <v>17</v>
       </c>
@@ -5041,25 +5665,27 @@
         <v>34</v>
       </c>
       <c r="P90" s="6">
-        <v>42279.708333333299</v>
+        <v>42279.7083333333</v>
       </c>
       <c r="Q90" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+      <selection activeCell="A29" sqref="$A29:$XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -5067,6 +5693,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>